<commit_message>
feat(koc): Improvements from excel file
</commit_message>
<xml_diff>
--- a/KOCModel/Workbooks/main.xlsx
+++ b/KOCModel/Workbooks/main.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17766"/>
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28827"/>
   <workbookPr dateCompatibility="0" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nemanja Pavlovic\Documents\visual studio 2015\Projects\KOCModel\KOCModel\Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\VS ME Dropbox\Nenad Mandich\Work\Jobs\2024\Kuwait - K24000\K24007-GER-PX-001\Guidelines update\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{7DE6A0C2-4701-445E-AFFC-0A0708CBFFE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="90" windowWidth="19815" windowHeight="7875" activeTab="1"/>
+    <workbookView xWindow="38280" yWindow="1890" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,17 +23,28 @@
   <definedNames>
     <definedName name="material">'[1]Max hole size'!$G$5:$G$19</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="453" uniqueCount="183">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="474" uniqueCount="208">
   <si>
     <t xml:space="preserve">Name </t>
   </si>
@@ -331,87 +343,9 @@
     <t>B4</t>
   </si>
   <si>
-    <t>Hydrocarbon wellhead</t>
-  </si>
-  <si>
-    <t>Water wellhead</t>
-  </si>
-  <si>
-    <t>Gas Separation/Unfired Equipment</t>
-  </si>
-  <si>
-    <t>Fired heaters (with flame arrestor)</t>
-  </si>
-  <si>
-    <t>Fired heaters (without flame arrestor)</t>
-  </si>
-  <si>
-    <t>Crude oil storage tank</t>
-  </si>
-  <si>
-    <t>Produced water storage tank</t>
-  </si>
-  <si>
-    <t>Gas compressors (field development)</t>
-  </si>
-  <si>
-    <t>Gas compressors (vapour recovery)</t>
-  </si>
-  <si>
-    <t>Metering pumps (internal comb diver)</t>
-  </si>
-  <si>
-    <t>Truck (un)loading (crude/condensate)</t>
-  </si>
-  <si>
-    <t>HC pits (normally burning)</t>
-  </si>
-  <si>
-    <t>HC pits (not normally burning)</t>
-  </si>
-  <si>
-    <t>Emergency pits</t>
-  </si>
-  <si>
-    <t>Low volatity storage (or &lt;5m3)</t>
-  </si>
-  <si>
-    <t>Service building</t>
-  </si>
-  <si>
-    <t>Unclassified switchgear and instrument rooms</t>
-  </si>
-  <si>
-    <t>Transformers</t>
-  </si>
-  <si>
-    <t>Electric power lines above ground</t>
-  </si>
-  <si>
-    <t>Public roads</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
-    <t>Hydraulic pumps (gas engine driven)</t>
-  </si>
-  <si>
-    <t>Metering pumps (produced HC)</t>
-  </si>
-  <si>
-    <t>Hydraulic pumps (electric motor driven)</t>
-  </si>
-  <si>
-    <t>Truck (un)loading (water/sump pits)</t>
-  </si>
-  <si>
-    <t>nr</t>
-  </si>
-  <si>
-    <t>0.5D</t>
-  </si>
-  <si>
     <t>HP Slug catcher</t>
   </si>
   <si>
@@ -532,9 +466,6 @@
     <t>To be determined by other requirements (e.g. operational, maintenance, inspection, etc.)</t>
   </si>
   <si>
-    <t>Refer Section 5.5.1.4</t>
-  </si>
-  <si>
     <t>No requirement / not relevant</t>
   </si>
   <si>
@@ -581,16 +512,172 @@
   </si>
   <si>
     <t>Flow or storage tanks from oil well</t>
+  </si>
+  <si>
+    <t>Wells, Field Development Equipment and Infrastructure</t>
+  </si>
+  <si>
+    <t>Deep wells (NK Jurassic, SEK &amp; WK)</t>
+  </si>
+  <si>
+    <t>Conventional wells (NK, SEK, &amp; WK)</t>
+  </si>
+  <si>
+    <t>Heavy oil wells (NK)</t>
+  </si>
+  <si>
+    <t>Drilling flares and burn pits</t>
+  </si>
+  <si>
+    <t>Processing facility perimeter fence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Individual inter-field hydrocarbon processing equipment </t>
+  </si>
+  <si>
+    <t>(N10)</t>
+  </si>
+  <si>
+    <t>30/15 (N1)</t>
+  </si>
+  <si>
+    <t>5/10 (N1)</t>
+  </si>
+  <si>
+    <t>50-75 (N4)</t>
+  </si>
+  <si>
+    <t>(N3)</t>
+  </si>
+  <si>
+    <t>(N11)</t>
+  </si>
+  <si>
+    <t>60-80 (N4)</t>
+  </si>
+  <si>
+    <t>50-70 (N4)</t>
+  </si>
+  <si>
+    <t>(N5)</t>
+  </si>
+  <si>
+    <t>30-40 (N4)</t>
+  </si>
+  <si>
+    <t>40-50 (N4)</t>
+  </si>
+  <si>
+    <t>75-100 (N4)</t>
+  </si>
+  <si>
+    <t>60-90 (N4)</t>
+  </si>
+  <si>
+    <t>(N6)</t>
+  </si>
+  <si>
+    <t>(N7)</t>
+  </si>
+  <si>
+    <t>50-60 (N4)</t>
+  </si>
+  <si>
+    <t>(N8)</t>
+  </si>
+  <si>
+    <t>30/40 (N2)</t>
+  </si>
+  <si>
+    <t>(N9)</t>
+  </si>
+  <si>
+    <t>Adjacent individual well (hydrocarbons)</t>
+  </si>
+  <si>
+    <t>Adjacent multi-well pad well (hydrocarbons)</t>
+  </si>
+  <si>
+    <t>Adjacent well (non-flammable water-based fluids -water, brine, dilute effluents)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hydrocarbon processing equipment </t>
+  </si>
+  <si>
+    <t>Above-ground powerlines (N12)</t>
+  </si>
+  <si>
+    <t>Above-ground hydrocarbon flowlines/pipelines</t>
+  </si>
+  <si>
+    <t>Below-ground hydrocarbon flowlines/pipelines</t>
+  </si>
+  <si>
+    <t>Above-ground utility pipelines (N12)</t>
+  </si>
+  <si>
+    <t>Road (within KOC concession area boundary fence)</t>
+  </si>
+  <si>
+    <t>Camps, rig site offices and other occupied areas and buildings (N10)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equipment with flammable/combustible liquid </t>
+  </si>
+  <si>
+    <t>Crude oil storage facilities</t>
+  </si>
+  <si>
+    <t>Water storage</t>
+  </si>
+  <si>
+    <t>Chemical storage</t>
+  </si>
+  <si>
+    <t>Un-classified electrical switchgear</t>
+  </si>
+  <si>
+    <t>Electrical transformers</t>
+  </si>
+  <si>
+    <t>Electrical power generators</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Service/unoccupied building </t>
+  </si>
+  <si>
+    <t>Welding (hot work) shop</t>
+  </si>
+  <si>
+    <t>Spark-generating or fired equipment</t>
+  </si>
+  <si>
+    <t>Blowout preventer (BOP) control unit/accumulator</t>
+  </si>
+  <si>
+    <t>Public infrastructure (roads and buildings)</t>
+  </si>
+  <si>
+    <t>4.7 kW/m2</t>
+  </si>
+  <si>
+    <t>1.6 kW/m2</t>
+  </si>
+  <si>
+    <t>1.2 kW/m2</t>
+  </si>
+  <si>
+    <t>Refer Section 5.5.1.6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -622,23 +709,37 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -668,7 +769,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -719,12 +820,28 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
@@ -767,13 +884,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8197" name="Button 5">
+        <xdr:cNvPr id="9221" name="Button 5">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s2053"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{424E8558-BDB0-4F21-9170-07A9BCB7CC22}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AB7D2976-E5A9-1F07-5FA5-3393FF1C3904}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -808,18 +925,19 @@
         </a:extLst>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
             <a:defRPr sz="1000"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="sr-Latn-RS" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0%">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:t>Start Model</a:t>
@@ -844,13 +962,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8198" name="Button 6">
+        <xdr:cNvPr id="9222" name="Button 6">
           <a:extLst>
             <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
               <a14:compatExt xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" spid="_x0000_s2054"/>
             </a:ext>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F87C90-B612-4683-A180-FE029A23CCE4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76AA0B12-A10F-FE42-2DAB-B67D29F2CECB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -885,18 +1003,19 @@
         </a:extLst>
       </xdr:spPr>
       <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="27432" rIns="27432" bIns="27432" anchor="ctr" upright="1"/>
+        <a:bodyPr vertOverflow="clip" wrap="square" lIns="27432" tIns="22860" rIns="27432" bIns="22860" anchor="ctr" upright="1"/>
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="ctr" rtl="0">
             <a:defRPr sz="1000"/>
           </a:pPr>
           <a:r>
-            <a:rPr lang="sr-Latn-RS" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0%">
+            <a:rPr lang="en-AU" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0%">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
               <a:latin typeface="Calibri"/>
+              <a:ea typeface="Calibri"/>
               <a:cs typeface="Calibri"/>
             </a:rPr>
             <a:t>Exit Model</a:t>
@@ -906,11 +1025,60 @@
     </xdr:sp>
     <xdr:clientData fPrintsWithSheet="0"/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>193001</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>22679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>180878</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43B611B1-0DF2-C662-3F25-EFBF11D39779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15296930" y="16544018"/>
+          <a:ext cx="3050034" cy="5612396"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Chart1"/>
@@ -1015,9 +1183,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1055,9 +1223,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1090,26 +1258,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1142,26 +1293,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1334,7 +1468,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
@@ -1352,22 +1486,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:xdr="http://purl.oclc.org/ooxml/drawingml/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:Y185"/>
+  <dimension ref="A1:S185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A152" workbookViewId="0">
-      <selection activeCell="D181" sqref="D181"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>20</v>
@@ -1535,7 +1672,7 @@
         <v>0</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>143</v>
+        <v>117</v>
       </c>
       <c r="C21" s="2"/>
     </row>
@@ -1666,7 +1803,7 @@
         <v>54</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>142</v>
+        <v>116</v>
       </c>
       <c r="C41" s="1"/>
     </row>
@@ -2943,7 +3080,7 @@
       </c>
     </row>
     <row r="80" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A80" s="17">
+      <c r="A80">
         <f>IF(B80="","Temp",B80)</f>
         <v>42442</v>
       </c>
@@ -2951,1014 +3088,595 @@
         <v>2016-03-13</v>
       </c>
     </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>99</v>
-      </c>
-      <c r="B85" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="83" spans="1:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="19"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="19"/>
+      <c r="D83" s="19"/>
+      <c r="E83" s="19"/>
+      <c r="F83" s="19"/>
+      <c r="G83" s="19"/>
+      <c r="H83" s="18"/>
+    </row>
+    <row r="84" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="B84" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="C84" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="D84" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F84" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G84" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="H84" s="18"/>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="B85" s="22">
+        <v>30</v>
+      </c>
+      <c r="C85" s="22">
+        <v>30</v>
+      </c>
+      <c r="D85" s="22">
+        <v>30</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F85" s="22">
+        <v>50</v>
+      </c>
+      <c r="G85" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="B86" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="C86" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="D86" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="E86" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F86" s="22">
+        <v>50</v>
+      </c>
+      <c r="G86" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="B87" s="22">
+        <v>30</v>
+      </c>
+      <c r="C87" s="22">
+        <v>30</v>
+      </c>
+      <c r="D87" s="22">
+        <v>30</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="F87" s="22">
+        <v>50</v>
+      </c>
+      <c r="G87" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="B88" s="22">
+        <v>70</v>
+      </c>
+      <c r="C88" s="22">
+        <v>50</v>
+      </c>
+      <c r="D88" s="22">
+        <v>35</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F88" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="G88" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="B89" s="22">
         <v>100</v>
       </c>
-      <c r="B86" t="s">
-        <v>124</v>
-      </c>
-      <c r="C86" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>101</v>
-      </c>
-      <c r="B87">
+      <c r="C89" s="22">
+        <v>75</v>
+      </c>
+      <c r="D89" s="22">
+        <v>50</v>
+      </c>
+      <c r="E89" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="F89" s="22">
+        <v>80</v>
+      </c>
+      <c r="G89" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="B90" s="22">
+        <v>50</v>
+      </c>
+      <c r="C90" s="22">
+        <v>45</v>
+      </c>
+      <c r="D90" s="22">
+        <v>40</v>
+      </c>
+      <c r="E90" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F90" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="G90" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="B91" s="22">
+        <v>80</v>
+      </c>
+      <c r="C91" s="22">
+        <v>60</v>
+      </c>
+      <c r="D91" s="22">
+        <v>50</v>
+      </c>
+      <c r="E91" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="F91" s="22">
+        <v>50</v>
+      </c>
+      <c r="G91" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B92" s="22">
+        <v>70</v>
+      </c>
+      <c r="C92" s="22">
+        <v>50</v>
+      </c>
+      <c r="D92" s="22">
+        <v>35</v>
+      </c>
+      <c r="E92" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F92" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G92" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" s="21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B93" s="22">
+        <v>35</v>
+      </c>
+      <c r="C93" s="22">
+        <v>25</v>
+      </c>
+      <c r="D93" s="22">
+        <v>20</v>
+      </c>
+      <c r="E93" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="F93" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="G93" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" s="21" t="s">
+        <v>189</v>
+      </c>
+      <c r="B94" s="22">
         <v>30</v>
       </c>
-      <c r="C87">
+      <c r="C94" s="22">
         <v>30</v>
       </c>
-      <c r="D87" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>102</v>
-      </c>
-      <c r="B88">
+      <c r="D94" s="22">
         <v>30</v>
       </c>
-      <c r="C88">
+      <c r="E94" s="22" t="s">
+        <v>173</v>
+      </c>
+      <c r="F94" s="22">
+        <v>20</v>
+      </c>
+      <c r="G94" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="B95" s="22">
+        <v>100</v>
+      </c>
+      <c r="C95" s="22">
+        <v>75</v>
+      </c>
+      <c r="D95" s="22">
+        <v>50</v>
+      </c>
+      <c r="E95" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="F95" s="22">
+        <v>5</v>
+      </c>
+      <c r="G95" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" s="21" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" s="22">
+        <v>90</v>
+      </c>
+      <c r="C96" s="22">
+        <v>60</v>
+      </c>
+      <c r="D96" s="22">
+        <v>55</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="F96" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="G96" s="22" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A97" s="21" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="22">
+        <v>40</v>
+      </c>
+      <c r="C97" s="22">
+        <v>30</v>
+      </c>
+      <c r="D97" s="22">
         <v>25</v>
       </c>
-      <c r="D88">
+      <c r="E97" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="F97" s="22">
         <v>30</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>103</v>
-      </c>
-      <c r="B89">
-        <v>50</v>
-      </c>
-      <c r="C89">
+      <c r="G97" s="22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="98" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A98" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B98" s="22">
+        <v>70</v>
+      </c>
+      <c r="C98" s="22">
+        <v>60</v>
+      </c>
+      <c r="D98" s="22">
+        <v>50</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="F98" s="22">
+        <v>60</v>
+      </c>
+      <c r="G98" s="22" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="99" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A99" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="B99" s="22">
+        <v>50</v>
+      </c>
+      <c r="C99" s="22">
+        <v>50</v>
+      </c>
+      <c r="D99" s="22">
+        <v>50</v>
+      </c>
+      <c r="E99" s="22">
+        <v>60</v>
+      </c>
+      <c r="F99" s="22">
         <v>30</v>
       </c>
-      <c r="D89">
-        <v>50</v>
-      </c>
-      <c r="E89">
-        <v>50</v>
-      </c>
-      <c r="F89">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>104</v>
-      </c>
-      <c r="B90">
-        <v>50</v>
-      </c>
-      <c r="C90">
-        <v>50</v>
-      </c>
-      <c r="D90">
-        <v>15</v>
-      </c>
-      <c r="E90">
+      <c r="G99" s="22">
         <v>30</v>
       </c>
-      <c r="F90">
-        <v>50</v>
-      </c>
-      <c r="G90" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>105</v>
-      </c>
-      <c r="B91">
+    </row>
+    <row r="100" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A100" s="21" t="s">
+        <v>195</v>
+      </c>
+      <c r="B100" s="22">
         <v>30</v>
       </c>
-      <c r="C91">
-        <v>15</v>
-      </c>
-      <c r="D91">
-        <v>10</v>
-      </c>
-      <c r="E91">
-        <v>25</v>
-      </c>
-      <c r="F91">
+      <c r="C100" s="22">
+        <v>30</v>
+      </c>
+      <c r="D100" s="22">
+        <v>30</v>
+      </c>
+      <c r="E100" s="22">
+        <v>60</v>
+      </c>
+      <c r="F100" s="22">
+        <v>30</v>
+      </c>
+      <c r="G100" s="22">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A101" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="B101" s="22">
+        <v>30</v>
+      </c>
+      <c r="C101" s="22">
+        <v>30</v>
+      </c>
+      <c r="D101" s="22">
+        <v>30</v>
+      </c>
+      <c r="E101" s="22">
+        <v>50</v>
+      </c>
+      <c r="F101" s="22">
+        <v>20</v>
+      </c>
+      <c r="G101" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A102" s="21" t="s">
+        <v>197</v>
+      </c>
+      <c r="B102" s="22">
+        <v>50</v>
+      </c>
+      <c r="C102" s="22">
+        <v>45</v>
+      </c>
+      <c r="D102" s="22">
         <v>40</v>
       </c>
-      <c r="G91" t="s">
-        <v>125</v>
-      </c>
-      <c r="H91" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>106</v>
-      </c>
-      <c r="B92">
-        <v>50</v>
-      </c>
-      <c r="C92">
+      <c r="E102" s="22">
+        <v>50</v>
+      </c>
+      <c r="F102" s="22">
         <v>30</v>
       </c>
-      <c r="D92">
-        <v>15</v>
-      </c>
-      <c r="E92">
+      <c r="G102" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="103" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A103" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B103" s="22">
+        <v>45</v>
+      </c>
+      <c r="C103" s="22">
+        <v>40</v>
+      </c>
+      <c r="D103" s="22">
+        <v>35</v>
+      </c>
+      <c r="E103" s="22">
+        <v>50</v>
+      </c>
+      <c r="F103" s="22">
         <v>30</v>
       </c>
-      <c r="F92">
-        <v>50</v>
-      </c>
-      <c r="G92">
-        <v>50</v>
-      </c>
-      <c r="H92">
+      <c r="G103" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A104" s="21" t="s">
+        <v>199</v>
+      </c>
+      <c r="B104" s="22">
+        <v>45</v>
+      </c>
+      <c r="C104" s="22">
+        <v>40</v>
+      </c>
+      <c r="D104" s="22">
+        <v>35</v>
+      </c>
+      <c r="E104" s="22">
+        <v>50</v>
+      </c>
+      <c r="F104" s="22">
         <v>30</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>107</v>
-      </c>
-      <c r="B93">
-        <v>30</v>
-      </c>
-      <c r="C93">
-        <v>30</v>
-      </c>
-      <c r="D93">
-        <v>10</v>
-      </c>
-      <c r="E93">
-        <v>25</v>
-      </c>
-      <c r="F93">
+      <c r="G104" s="22">
         <v>40</v>
       </c>
-      <c r="G93">
-        <v>10</v>
-      </c>
-      <c r="H93">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>121</v>
-      </c>
-      <c r="B94">
-        <v>30</v>
-      </c>
-      <c r="C94">
-        <v>30</v>
-      </c>
-      <c r="D94">
-        <v>15</v>
-      </c>
-      <c r="E94">
-        <v>30</v>
-      </c>
-      <c r="F94">
-        <v>50</v>
-      </c>
-      <c r="G94">
-        <v>15</v>
-      </c>
-      <c r="H94">
-        <v>10</v>
-      </c>
-      <c r="I94">
-        <v>10</v>
-      </c>
-      <c r="J94">
-        <v>10</v>
-      </c>
-      <c r="K94" t="s">
-        <v>124</v>
-      </c>
-      <c r="L94" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>108</v>
-      </c>
-      <c r="B95">
-        <v>30</v>
-      </c>
-      <c r="C95">
-        <v>30</v>
-      </c>
-      <c r="D95">
-        <v>15</v>
-      </c>
-      <c r="E95">
-        <v>15</v>
-      </c>
-      <c r="F95">
-        <v>15</v>
-      </c>
-      <c r="G95">
-        <v>15</v>
-      </c>
-      <c r="H95">
-        <v>10</v>
-      </c>
-      <c r="I95">
-        <v>15</v>
-      </c>
-      <c r="J95">
-        <v>15</v>
-      </c>
-      <c r="K95" t="s">
-        <v>124</v>
-      </c>
-      <c r="L95" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>120</v>
-      </c>
-      <c r="B96">
-        <v>50</v>
-      </c>
-      <c r="C96">
-        <v>30</v>
-      </c>
-      <c r="D96">
-        <v>30</v>
-      </c>
-      <c r="E96">
-        <v>30</v>
-      </c>
-      <c r="F96">
-        <v>50</v>
-      </c>
-      <c r="G96">
-        <v>50</v>
-      </c>
-      <c r="H96">
-        <v>30</v>
-      </c>
-      <c r="I96">
-        <v>50</v>
-      </c>
-      <c r="J96">
-        <v>50</v>
-      </c>
-      <c r="K96">
-        <v>30</v>
-      </c>
-      <c r="L96">
-        <v>30</v>
-      </c>
-      <c r="M96" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="97" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>122</v>
-      </c>
-      <c r="B97">
-        <v>30</v>
-      </c>
-      <c r="C97">
-        <v>30</v>
-      </c>
-      <c r="D97">
-        <v>15</v>
-      </c>
-      <c r="E97">
-        <v>30</v>
-      </c>
-      <c r="F97">
-        <v>50</v>
-      </c>
-      <c r="G97">
-        <v>30</v>
-      </c>
-      <c r="H97">
-        <v>15</v>
-      </c>
-      <c r="I97">
-        <v>30</v>
-      </c>
-      <c r="J97">
-        <v>30</v>
-      </c>
-      <c r="K97">
-        <v>30</v>
-      </c>
-      <c r="L97">
-        <v>30</v>
-      </c>
-      <c r="M97">
-        <v>30</v>
-      </c>
-      <c r="N97" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="98" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>109</v>
-      </c>
-      <c r="B98">
-        <v>30</v>
-      </c>
-      <c r="C98">
-        <v>30</v>
-      </c>
-      <c r="D98">
-        <v>30</v>
-      </c>
-      <c r="E98">
-        <v>30</v>
-      </c>
-      <c r="F98">
-        <v>50</v>
-      </c>
-      <c r="G98">
-        <v>50</v>
-      </c>
-      <c r="H98">
-        <v>30</v>
-      </c>
-      <c r="I98">
-        <v>50</v>
-      </c>
-      <c r="J98">
-        <v>50</v>
-      </c>
-      <c r="K98" t="s">
-        <v>124</v>
-      </c>
-      <c r="L98" t="s">
-        <v>124</v>
-      </c>
-      <c r="M98">
-        <v>50</v>
-      </c>
-      <c r="N98">
-        <v>50</v>
-      </c>
-      <c r="O98" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="99" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>123</v>
-      </c>
-      <c r="B99">
-        <v>30</v>
-      </c>
-      <c r="C99">
-        <v>30</v>
-      </c>
-      <c r="D99">
-        <v>15</v>
-      </c>
-      <c r="E99">
-        <v>30</v>
-      </c>
-      <c r="F99">
-        <v>50</v>
-      </c>
-      <c r="G99">
-        <v>30</v>
-      </c>
-      <c r="H99">
-        <v>15</v>
-      </c>
-      <c r="I99">
-        <v>30</v>
-      </c>
-      <c r="J99">
-        <v>30</v>
-      </c>
-      <c r="K99">
-        <v>30</v>
-      </c>
-      <c r="L99">
-        <v>30</v>
-      </c>
-      <c r="M99">
-        <v>50</v>
-      </c>
-      <c r="N99">
-        <v>50</v>
-      </c>
-      <c r="O99">
-        <v>10</v>
-      </c>
-      <c r="P99" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="100" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>110</v>
-      </c>
-      <c r="B100">
-        <v>50</v>
-      </c>
-      <c r="C100">
-        <v>30</v>
-      </c>
-      <c r="D100">
-        <v>50</v>
-      </c>
-      <c r="E100">
-        <v>50</v>
-      </c>
-      <c r="F100">
-        <v>50</v>
-      </c>
-      <c r="G100">
-        <v>50</v>
-      </c>
-      <c r="H100">
-        <v>30</v>
-      </c>
-      <c r="I100">
-        <v>50</v>
-      </c>
-      <c r="J100">
-        <v>50</v>
-      </c>
-      <c r="K100" t="s">
-        <v>124</v>
-      </c>
-      <c r="L100" t="s">
-        <v>124</v>
-      </c>
-      <c r="M100">
-        <v>50</v>
-      </c>
-      <c r="N100">
-        <v>50</v>
-      </c>
-      <c r="O100">
-        <v>50</v>
-      </c>
-      <c r="P100">
-        <v>15</v>
-      </c>
-      <c r="Q100">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="101" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>111</v>
-      </c>
-      <c r="B101">
-        <v>30</v>
-      </c>
-      <c r="C101">
-        <v>30</v>
-      </c>
-      <c r="D101">
-        <v>30</v>
-      </c>
-      <c r="E101">
-        <v>30</v>
-      </c>
-      <c r="F101">
-        <v>50</v>
-      </c>
-      <c r="G101">
-        <v>30</v>
-      </c>
-      <c r="H101">
-        <v>25</v>
-      </c>
-      <c r="I101">
-        <v>50</v>
-      </c>
-      <c r="J101">
-        <v>30</v>
-      </c>
-      <c r="K101">
-        <v>15</v>
-      </c>
-      <c r="L101">
-        <v>10</v>
-      </c>
-      <c r="M101">
-        <v>50</v>
-      </c>
-      <c r="N101">
-        <v>30</v>
-      </c>
-      <c r="O101">
-        <v>50</v>
-      </c>
-      <c r="P101">
-        <v>15</v>
-      </c>
-      <c r="Q101">
-        <v>30</v>
-      </c>
-      <c r="R101">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="102" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>112</v>
-      </c>
-      <c r="B102">
-        <v>30</v>
-      </c>
-      <c r="C102">
-        <v>30</v>
-      </c>
-      <c r="D102">
-        <v>15</v>
-      </c>
-      <c r="E102">
-        <v>15</v>
-      </c>
-      <c r="F102">
-        <v>30</v>
-      </c>
-      <c r="G102">
-        <v>15</v>
-      </c>
-      <c r="H102">
-        <v>10</v>
-      </c>
-      <c r="I102">
-        <v>30</v>
-      </c>
-      <c r="J102">
-        <v>15</v>
-      </c>
-      <c r="K102">
-        <v>15</v>
-      </c>
-      <c r="L102">
-        <v>10</v>
-      </c>
-      <c r="M102">
-        <v>30</v>
-      </c>
-      <c r="N102">
-        <v>15</v>
-      </c>
-      <c r="O102">
-        <v>30</v>
-      </c>
-      <c r="P102">
-        <v>10</v>
-      </c>
-      <c r="Q102">
-        <v>50</v>
-      </c>
-      <c r="R102">
-        <v>30</v>
-      </c>
-      <c r="S102" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="103" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>113</v>
-      </c>
-      <c r="B103">
-        <v>15</v>
-      </c>
-      <c r="C103">
-        <v>15</v>
-      </c>
-      <c r="D103">
-        <v>10</v>
-      </c>
-      <c r="E103">
-        <v>25</v>
-      </c>
-      <c r="F103">
-        <v>30</v>
-      </c>
-      <c r="G103">
-        <v>10</v>
-      </c>
-      <c r="H103">
-        <v>10</v>
-      </c>
-      <c r="I103">
-        <v>15</v>
-      </c>
-      <c r="J103">
-        <v>10</v>
-      </c>
-      <c r="K103">
-        <v>10</v>
-      </c>
-      <c r="L103">
-        <v>10</v>
-      </c>
-      <c r="M103">
-        <v>10</v>
-      </c>
-      <c r="N103">
-        <v>10</v>
-      </c>
-      <c r="O103">
-        <v>10</v>
-      </c>
-      <c r="P103">
-        <v>10</v>
-      </c>
-      <c r="Q103">
-        <v>50</v>
-      </c>
-      <c r="R103">
-        <v>30</v>
-      </c>
-      <c r="S103">
-        <v>50</v>
-      </c>
-      <c r="T103" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="104" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>114</v>
-      </c>
-      <c r="B104">
-        <v>30</v>
-      </c>
-      <c r="C104">
-        <v>30</v>
-      </c>
-      <c r="D104">
-        <v>30</v>
-      </c>
-      <c r="E104">
-        <v>30</v>
-      </c>
-      <c r="F104">
-        <v>30</v>
-      </c>
-      <c r="G104">
-        <v>50</v>
-      </c>
-      <c r="H104">
-        <v>30</v>
-      </c>
-      <c r="I104">
-        <v>50</v>
-      </c>
-      <c r="J104">
-        <v>30</v>
-      </c>
-      <c r="K104">
-        <v>30</v>
-      </c>
-      <c r="L104">
-        <v>15</v>
-      </c>
-      <c r="M104">
-        <v>50</v>
-      </c>
-      <c r="N104">
-        <v>50</v>
-      </c>
-      <c r="O104">
-        <v>30</v>
-      </c>
-      <c r="P104">
-        <v>30</v>
-      </c>
-      <c r="Q104">
-        <v>50</v>
-      </c>
-      <c r="R104">
-        <v>30</v>
-      </c>
-      <c r="S104">
-        <v>50</v>
-      </c>
-      <c r="T104">
-        <v>10</v>
-      </c>
-      <c r="U104" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="105" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>115</v>
-      </c>
-      <c r="B105">
-        <v>30</v>
-      </c>
-      <c r="C105">
-        <v>15</v>
-      </c>
-      <c r="D105">
-        <v>10</v>
-      </c>
-      <c r="E105">
-        <v>10</v>
-      </c>
-      <c r="F105">
-        <v>10</v>
-      </c>
-      <c r="G105">
-        <v>15</v>
-      </c>
-      <c r="H105">
-        <v>10</v>
-      </c>
-      <c r="I105">
-        <v>10</v>
-      </c>
-      <c r="J105">
-        <v>3</v>
-      </c>
-      <c r="K105">
-        <v>3</v>
-      </c>
-      <c r="L105">
-        <v>3</v>
-      </c>
-      <c r="M105">
-        <v>30</v>
-      </c>
-      <c r="N105">
-        <v>15</v>
-      </c>
-      <c r="O105">
-        <v>15</v>
-      </c>
-      <c r="P105">
-        <v>10</v>
-      </c>
-      <c r="Q105">
-        <v>50</v>
-      </c>
-      <c r="R105">
-        <v>30</v>
-      </c>
-      <c r="S105">
-        <v>50</v>
-      </c>
-      <c r="T105">
-        <v>3</v>
-      </c>
-      <c r="U105" t="s">
-        <v>124</v>
-      </c>
-      <c r="V105" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="106" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
-        <v>116</v>
-      </c>
-      <c r="B106">
-        <v>50</v>
-      </c>
-      <c r="C106">
-        <v>50</v>
-      </c>
-      <c r="D106">
-        <v>30</v>
-      </c>
-      <c r="E106">
-        <v>30</v>
-      </c>
-      <c r="F106">
-        <v>30</v>
-      </c>
-      <c r="G106">
-        <v>30</v>
-      </c>
-      <c r="H106">
-        <v>25</v>
-      </c>
-      <c r="I106">
-        <v>30</v>
-      </c>
-      <c r="J106">
-        <v>25</v>
-      </c>
-      <c r="K106">
-        <v>15</v>
-      </c>
-      <c r="L106">
-        <v>15</v>
-      </c>
-      <c r="M106">
-        <v>50</v>
-      </c>
-      <c r="N106">
-        <v>30</v>
-      </c>
-      <c r="O106">
-        <v>30</v>
-      </c>
-      <c r="P106">
-        <v>25</v>
-      </c>
-      <c r="Q106">
-        <v>50</v>
-      </c>
-      <c r="R106">
-        <v>15</v>
-      </c>
-      <c r="S106">
-        <v>50</v>
-      </c>
-      <c r="T106">
-        <v>15</v>
-      </c>
-      <c r="U106">
-        <v>10</v>
-      </c>
-      <c r="V106">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="107" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
-        <v>117</v>
-      </c>
-      <c r="B107">
-        <v>50</v>
-      </c>
-      <c r="C107">
-        <v>50</v>
-      </c>
-      <c r="D107">
-        <v>15</v>
-      </c>
-      <c r="E107">
-        <v>15</v>
-      </c>
-      <c r="F107">
-        <v>15</v>
-      </c>
-      <c r="G107">
-        <v>10</v>
-      </c>
-      <c r="H107">
-        <v>10</v>
-      </c>
-      <c r="I107">
-        <v>10</v>
-      </c>
-      <c r="J107">
-        <v>10</v>
-      </c>
-      <c r="K107">
-        <v>10</v>
-      </c>
-      <c r="L107">
-        <v>10</v>
-      </c>
-      <c r="M107">
-        <v>15</v>
-      </c>
-      <c r="N107">
-        <v>15</v>
-      </c>
-      <c r="O107">
-        <v>15</v>
-      </c>
-      <c r="P107">
-        <v>15</v>
-      </c>
-      <c r="Q107">
-        <v>30</v>
-      </c>
-      <c r="R107">
-        <v>10</v>
-      </c>
-      <c r="S107">
-        <v>30</v>
-      </c>
-      <c r="T107">
-        <v>10</v>
-      </c>
-      <c r="U107">
-        <v>10</v>
-      </c>
-      <c r="V107" t="s">
-        <v>124</v>
-      </c>
-      <c r="W107" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="108" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>118</v>
-      </c>
-      <c r="B108">
-        <v>50</v>
-      </c>
-      <c r="C108">
-        <v>50</v>
-      </c>
-      <c r="D108">
-        <v>30</v>
-      </c>
-      <c r="E108">
-        <v>30</v>
-      </c>
-      <c r="F108">
-        <v>30</v>
-      </c>
-      <c r="G108">
-        <v>50</v>
-      </c>
-      <c r="H108">
-        <v>30</v>
-      </c>
-      <c r="I108">
-        <v>30</v>
-      </c>
-      <c r="J108">
-        <v>30</v>
-      </c>
-      <c r="K108">
-        <v>15</v>
-      </c>
-      <c r="L108">
-        <v>15</v>
-      </c>
-      <c r="M108">
-        <v>50</v>
-      </c>
-      <c r="N108">
-        <v>50</v>
-      </c>
-      <c r="O108">
-        <v>30</v>
-      </c>
-      <c r="P108">
-        <v>30</v>
-      </c>
-      <c r="Q108">
-        <v>50</v>
-      </c>
-      <c r="R108">
-        <v>30</v>
-      </c>
-      <c r="S108">
-        <v>50</v>
-      </c>
-      <c r="T108">
-        <v>15</v>
-      </c>
-      <c r="U108">
-        <v>10</v>
-      </c>
-      <c r="V108">
-        <v>15</v>
-      </c>
-      <c r="W108" t="s">
-        <v>124</v>
-      </c>
-      <c r="X108">
-        <v>10</v>
-      </c>
-      <c r="Y108" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="110" spans="1:25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="105" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A105" s="21" t="s">
+        <v>200</v>
+      </c>
+      <c r="B105" s="22">
+        <v>45</v>
+      </c>
+      <c r="C105" s="22">
+        <v>45</v>
+      </c>
+      <c r="D105" s="22">
+        <v>45</v>
+      </c>
+      <c r="E105" s="22">
+        <v>50</v>
+      </c>
+      <c r="F105" s="22">
+        <v>45</v>
+      </c>
+      <c r="G105" s="22">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="106" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A106" s="21" t="s">
+        <v>201</v>
+      </c>
+      <c r="B106" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C106" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="D106" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="E106" s="22">
+        <v>50</v>
+      </c>
+      <c r="F106" s="22">
+        <v>50</v>
+      </c>
+      <c r="G106" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="107" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A107" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B107" s="22">
+        <v>50</v>
+      </c>
+      <c r="C107" s="22">
+        <v>45</v>
+      </c>
+      <c r="D107" s="22">
+        <v>40</v>
+      </c>
+      <c r="E107" s="22">
+        <v>50</v>
+      </c>
+      <c r="F107" s="22">
+        <v>50</v>
+      </c>
+      <c r="G107" s="22">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="108" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A108" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="B108" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C108" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="D108" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="F108" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="G108" s="22" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="110" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="B110" s="15">
         <v>70</v>
@@ -3977,9 +3695,9 @@
       <c r="N110" s="15"/>
       <c r="O110" s="15"/>
     </row>
-    <row r="111" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="B111" s="15">
         <v>70</v>
@@ -4000,9 +3718,9 @@
       <c r="N111" s="15"/>
       <c r="O111" s="15"/>
     </row>
-    <row r="112" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="B112" s="15">
         <v>70</v>
@@ -4027,7 +3745,7 @@
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="B113" s="15">
         <v>15</v>
@@ -4039,7 +3757,7 @@
         <v>15</v>
       </c>
       <c r="E113" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F113" s="15"/>
       <c r="G113" s="15"/>
@@ -4054,7 +3772,7 @@
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="B114" s="15">
         <v>15</v>
@@ -4066,10 +3784,10 @@
         <v>15</v>
       </c>
       <c r="E114" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="F114" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="G114" s="15"/>
       <c r="H114" s="15"/>
@@ -4083,7 +3801,7 @@
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>131</v>
+        <v>105</v>
       </c>
       <c r="B115" s="15">
         <v>70</v>
@@ -4114,7 +3832,7 @@
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>132</v>
+        <v>106</v>
       </c>
       <c r="B116" s="15">
         <v>70</v>
@@ -4147,7 +3865,7 @@
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>133</v>
+        <v>107</v>
       </c>
       <c r="B117" s="15">
         <v>70</v>
@@ -4182,7 +3900,7 @@
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>134</v>
+        <v>108</v>
       </c>
       <c r="B118" s="15">
         <v>70</v>
@@ -4219,7 +3937,7 @@
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>135</v>
+        <v>109</v>
       </c>
       <c r="B119" s="15">
         <v>70</v>
@@ -4258,7 +3976,7 @@
     </row>
     <row r="120" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="B120" s="15">
         <v>70</v>
@@ -4291,7 +4009,7 @@
         <v>60</v>
       </c>
       <c r="L120" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="M120" s="15"/>
       <c r="N120" s="15"/>
@@ -4299,7 +4017,7 @@
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B121" s="15">
         <v>70</v>
@@ -4335,16 +4053,16 @@
         <v>60</v>
       </c>
       <c r="M121" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="N121" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="O121" s="15"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B122" s="15">
         <v>70</v>
@@ -4380,16 +4098,16 @@
         <v>60</v>
       </c>
       <c r="M122" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="N122" s="15" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
       <c r="O122" s="15"/>
     </row>
     <row r="123" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B123" s="15">
         <v>85</v>
@@ -4436,7 +4154,7 @@
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B124" s="15">
         <v>70</v>
@@ -4483,7 +4201,7 @@
     </row>
     <row r="125" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B125" s="15">
         <v>85</v>
@@ -4529,58 +4247,86 @@
       </c>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B128" t="s">
-        <v>147</v>
-      </c>
-      <c r="C128" t="s">
-        <v>148</v>
-      </c>
-      <c r="D128" t="s">
-        <v>149</v>
+      <c r="A128" s="21"/>
+      <c r="B128" s="21" t="s">
+        <v>121</v>
+      </c>
+      <c r="C128" s="21" t="s">
+        <v>122</v>
+      </c>
+      <c r="D128" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="E128" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="F128" s="23" t="s">
+        <v>205</v>
+      </c>
+      <c r="G128" s="23" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="129" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="21" t="s">
+        <v>119</v>
+      </c>
+      <c r="B129" s="21">
+        <v>55</v>
+      </c>
+      <c r="C129" s="21">
+        <v>70</v>
+      </c>
+      <c r="D129" s="21">
+        <v>80</v>
+      </c>
+      <c r="E129" s="21">
+        <v>85</v>
+      </c>
+      <c r="F129" s="21">
+        <v>105</v>
+      </c>
+      <c r="G129" s="21">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A130" s="21" t="s">
+        <v>120</v>
+      </c>
+      <c r="B130" s="21">
+        <v>75</v>
+      </c>
+      <c r="C130" s="21">
+        <v>95</v>
+      </c>
+      <c r="D130" s="21">
+        <v>110</v>
+      </c>
+      <c r="E130" s="21">
+        <v>115</v>
+      </c>
+      <c r="F130" s="21">
         <v>145</v>
       </c>
-      <c r="B129">
-        <v>55</v>
-      </c>
-      <c r="C129">
-        <v>70</v>
-      </c>
-      <c r="D129">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="130" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>146</v>
-      </c>
-      <c r="B130">
-        <v>75</v>
-      </c>
-      <c r="C130">
-        <v>95</v>
-      </c>
-      <c r="D130">
-        <v>110</v>
+      <c r="G130" s="21">
+        <v>150</v>
       </c>
     </row>
     <row r="134" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B134" t="s">
-        <v>147</v>
+        <v>121</v>
       </c>
       <c r="C134" t="s">
-        <v>148</v>
+        <v>122</v>
       </c>
       <c r="D134" t="s">
-        <v>149</v>
+        <v>123</v>
       </c>
     </row>
     <row r="135" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>150</v>
+        <v>124</v>
       </c>
       <c r="B135">
         <v>30</v>
@@ -4594,7 +4340,7 @@
     </row>
     <row r="136" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>153</v>
+        <v>127</v>
       </c>
       <c r="B136">
         <v>18</v>
@@ -4608,7 +4354,7 @@
     </row>
     <row r="137" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>152</v>
+        <v>126</v>
       </c>
       <c r="B137">
         <v>10</v>
@@ -4622,7 +4368,7 @@
     </row>
     <row r="138" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="B138">
         <v>50</v>
@@ -4636,7 +4382,7 @@
     </row>
     <row r="139" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>154</v>
+        <v>128</v>
       </c>
       <c r="B139">
         <v>45</v>
@@ -4650,7 +4396,7 @@
     </row>
     <row r="140" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>155</v>
+        <v>129</v>
       </c>
       <c r="B140">
         <v>40</v>
@@ -4664,63 +4410,63 @@
     </row>
     <row r="144" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="C144" t="s">
-        <v>126</v>
+        <v>100</v>
       </c>
       <c r="D144" t="s">
-        <v>127</v>
+        <v>101</v>
       </c>
       <c r="E144" t="s">
-        <v>128</v>
+        <v>102</v>
       </c>
       <c r="F144" t="s">
-        <v>129</v>
+        <v>103</v>
       </c>
       <c r="G144" t="s">
-        <v>130</v>
+        <v>104</v>
       </c>
       <c r="H144" t="s">
+        <v>105</v>
+      </c>
+      <c r="I144" t="s">
+        <v>106</v>
+      </c>
+      <c r="J144" t="s">
+        <v>107</v>
+      </c>
+      <c r="K144" t="s">
+        <v>108</v>
+      </c>
+      <c r="L144" t="s">
         <v>131</v>
       </c>
-      <c r="I144" t="s">
+      <c r="M144" t="s">
         <v>132</v>
       </c>
-      <c r="J144" t="s">
+      <c r="N144" t="s">
         <v>133</v>
       </c>
-      <c r="K144" t="s">
+      <c r="O144" t="s">
+        <v>109</v>
+      </c>
+      <c r="P144" t="s">
+        <v>110</v>
+      </c>
+      <c r="Q144" t="s">
+        <v>111</v>
+      </c>
+      <c r="R144" t="s">
+        <v>112</v>
+      </c>
+      <c r="S144" t="s">
         <v>134</v>
-      </c>
-      <c r="L144" t="s">
-        <v>157</v>
-      </c>
-      <c r="M144" t="s">
-        <v>158</v>
-      </c>
-      <c r="N144" t="s">
-        <v>159</v>
-      </c>
-      <c r="O144" t="s">
-        <v>135</v>
-      </c>
-      <c r="P144" t="s">
-        <v>136</v>
-      </c>
-      <c r="Q144" t="s">
-        <v>137</v>
-      </c>
-      <c r="R144" t="s">
-        <v>138</v>
-      </c>
-      <c r="S144" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="145" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>156</v>
+        <v>130</v>
       </c>
       <c r="B145">
         <v>70</v>
@@ -4728,384 +4474,384 @@
     </row>
     <row r="146" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>126</v>
-      </c>
-      <c r="B146" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C146" s="18" t="s">
-        <v>165</v>
+        <v>100</v>
+      </c>
+      <c r="B146" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C146" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>127</v>
-      </c>
-      <c r="B147" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C147" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D147" s="18" t="s">
-        <v>165</v>
+        <v>101</v>
+      </c>
+      <c r="B147" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C147" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D147" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="148" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>128</v>
-      </c>
-      <c r="B148" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C148" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D148" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E148" s="18" t="s">
-        <v>165</v>
+        <v>102</v>
+      </c>
+      <c r="B148" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C148" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D148" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E148" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>129</v>
-      </c>
-      <c r="B149" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C149" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D149" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E149" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F149" s="18" t="s">
-        <v>165</v>
+        <v>103</v>
+      </c>
+      <c r="B149" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C149" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D149" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E149" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F149" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="150" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>130</v>
-      </c>
-      <c r="B150" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C150" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D150" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E150" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F150" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G150" s="18" t="s">
-        <v>165</v>
+        <v>104</v>
+      </c>
+      <c r="B150" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C150" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D150" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E150" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F150" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G150" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="151" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>131</v>
-      </c>
-      <c r="B151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G151" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H151" s="18" t="s">
-        <v>165</v>
+        <v>105</v>
+      </c>
+      <c r="B151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G151" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H151" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="152" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>132</v>
-      </c>
-      <c r="B152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H152" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I152" s="18" t="s">
-        <v>165</v>
+        <v>106</v>
+      </c>
+      <c r="B152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H152" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I152" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="153" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>133</v>
-      </c>
-      <c r="B153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I153" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J153" s="18" t="s">
-        <v>165</v>
+        <v>107</v>
+      </c>
+      <c r="B153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I153" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J153" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="154" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>134</v>
-      </c>
-      <c r="B154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J154" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="K154" s="18" t="s">
-        <v>165</v>
+        <v>108</v>
+      </c>
+      <c r="B154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J154" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K154" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="155" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>157</v>
-      </c>
-      <c r="B155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="K155" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="L155" s="18" t="s">
-        <v>165</v>
+        <v>131</v>
+      </c>
+      <c r="B155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K155" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L155" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="156" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>158</v>
-      </c>
-      <c r="B156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="K156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="L156" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="M156" s="18" t="s">
-        <v>165</v>
+        <v>132</v>
+      </c>
+      <c r="B156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L156" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M156" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="157" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>159</v>
-      </c>
-      <c r="B157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="K157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="L157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="M157" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N157" s="18" t="s">
-        <v>165</v>
+        <v>133</v>
+      </c>
+      <c r="B157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M157" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="N157" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="158" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>135</v>
-      </c>
-      <c r="B158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="C158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="D158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="E158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="F158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="H158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="I158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="J158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="K158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="L158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="M158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="N158" s="18" t="s">
-        <v>165</v>
-      </c>
-      <c r="O158" s="18" t="s">
-        <v>165</v>
+        <v>109</v>
+      </c>
+      <c r="B158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="C158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="D158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="E158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="F158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="G158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="H158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="I158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="J158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="K158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="L158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="M158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="N158" s="17" t="s">
+        <v>139</v>
+      </c>
+      <c r="O158" s="17" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="159" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>136</v>
+        <v>110</v>
       </c>
       <c r="B159">
         <v>50</v>
@@ -5150,12 +4896,12 @@
         <v>45</v>
       </c>
       <c r="P159" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="160" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>137</v>
+        <v>111</v>
       </c>
       <c r="B160">
         <v>60</v>
@@ -5203,12 +4949,12 @@
         <v>100</v>
       </c>
       <c r="Q160" t="s">
-        <v>167</v>
+        <v>140</v>
       </c>
     </row>
     <row r="161" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="B161">
         <v>60</v>
@@ -5260,67 +5006,67 @@
       </c>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>160</v>
-      </c>
-      <c r="B162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="C162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="D162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="F162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="G162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="H162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="I162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="J162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="K162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="L162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="M162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="N162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="O162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="P162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="R162" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="S162" s="18" t="s">
-        <v>166</v>
+      <c r="A162" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="C162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="D162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="E162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="F162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="G162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="H162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="I162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="J162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="K162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="L162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="M162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="N162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="O162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="P162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="Q162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="R162" s="24" t="s">
+        <v>207</v>
+      </c>
+      <c r="S162" s="24" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="163" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>135</v>
       </c>
       <c r="B163">
         <v>100</v>
@@ -5379,7 +5125,7 @@
     </row>
     <row r="164" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>136</v>
       </c>
       <c r="B164">
         <v>150</v>
@@ -5426,7 +5172,7 @@
       <c r="P164">
         <v>25</v>
       </c>
-      <c r="Q164">
+      <c r="Q164" s="21">
         <v>150</v>
       </c>
       <c r="R164">
@@ -5438,7 +5184,7 @@
     </row>
     <row r="165" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>137</v>
       </c>
       <c r="B165">
         <v>100</v>
@@ -5497,7 +5243,7 @@
     </row>
     <row r="166" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="B166">
         <v>150</v>
@@ -5545,15 +5291,18 @@
         <v>150</v>
       </c>
       <c r="Q166">
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="R166">
         <v>100</v>
       </c>
+      <c r="S166">
+        <v>100</v>
+      </c>
     </row>
     <row r="167" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="B167">
         <v>85</v>
@@ -5612,7 +5361,7 @@
     </row>
     <row r="168" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="B168">
         <v>150</v>
@@ -5671,15 +5420,15 @@
     </row>
     <row r="172" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>168</v>
+        <v>141</v>
       </c>
       <c r="B172" t="s">
-        <v>169</v>
+        <v>142</v>
       </c>
     </row>
     <row r="173" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>170</v>
+        <v>143</v>
       </c>
       <c r="B173">
         <v>60</v>
@@ -5687,7 +5436,7 @@
     </row>
     <row r="174" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>171</v>
+        <v>144</v>
       </c>
       <c r="B174">
         <v>30</v>
@@ -5695,7 +5444,7 @@
     </row>
     <row r="175" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>172</v>
+        <v>145</v>
       </c>
       <c r="B175">
         <v>60</v>
@@ -5703,7 +5452,7 @@
     </row>
     <row r="176" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>173</v>
+        <v>146</v>
       </c>
       <c r="B176">
         <v>60</v>
@@ -5711,7 +5460,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>174</v>
+        <v>147</v>
       </c>
       <c r="B177">
         <v>50</v>
@@ -5719,7 +5468,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="B178">
         <v>15</v>
@@ -5727,7 +5476,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="B179">
         <v>15</v>
@@ -5735,7 +5484,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>177</v>
+        <v>150</v>
       </c>
       <c r="B180">
         <v>15</v>
@@ -5743,7 +5492,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>178</v>
+        <v>151</v>
       </c>
       <c r="B181">
         <v>15</v>
@@ -5751,7 +5500,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>179</v>
+        <v>152</v>
       </c>
       <c r="B182">
         <v>300</v>
@@ -5759,7 +5508,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>180</v>
+        <v>153</v>
       </c>
       <c r="B183">
         <v>150</v>
@@ -5767,7 +5516,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>181</v>
+        <v>154</v>
       </c>
       <c r="B184">
         <v>150</v>
@@ -5775,7 +5524,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>182</v>
+        <v>155</v>
       </c>
       <c r="B185">
         <v>300</v>
@@ -5783,10 +5532,10 @@
     </row>
   </sheetData>
   <dataValidations disablePrompts="1" count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B47" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"GRE, Steel"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H53:Q53">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H53:Q53" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>$AC$15:$AC$18</formula1>
     </dataValidation>
   </dataValidations>
@@ -5799,7 +5548,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <controls>
-    <control shapeId="8197" r:id="rId4" name="Button 5">
+    <control shapeId="9221" r:id="rId4" name="Button 5">
       <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Macro2">
         <anchor moveWithCells="1" sizeWithCells="1">
           <from>
@@ -5817,7 +5566,7 @@
         </anchor>
       </controlPr>
     </control>
-    <control shapeId="8198" r:id="rId5" name="Button 6">
+    <control shapeId="9222" r:id="rId5" name="Button 6">
       <controlPr defaultSize="0" print="0" autoFill="0" autoPict="0" macro="[0]!Macro1">
         <anchor moveWithCells="1" sizeWithCells="1">
           <from>
@@ -5840,7 +5589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>